<commit_message>
Add terms data support
</commit_message>
<xml_diff>
--- a/deltas.xlsx
+++ b/deltas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projs\diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB7D9C0-BB7D-4060-BCE7-0FCE8DC34C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF70E8B-DEA1-44DE-859E-D736A2A772C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1755" windowWidth="24705" windowHeight="13605" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24705" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Токи и напряжения" sheetId="1" r:id="rId1"/>
@@ -21390,10 +21390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO3"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:AO3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21423,376 +21423,452 @@
     <col min="39" max="42" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="B32" s="6">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="B40" s="6">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="4">
-        <v>1</v>
-      </c>
-      <c r="O2" s="5">
-        <v>1</v>
-      </c>
-      <c r="P2" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>1</v>
-      </c>
-      <c r="R2" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" s="6">
-        <v>1</v>
-      </c>
-      <c r="T2" s="4">
-        <v>1</v>
-      </c>
-      <c r="U2" s="5">
-        <v>1</v>
-      </c>
-      <c r="V2" s="6">
-        <v>1</v>
-      </c>
-      <c r="W2" s="4">
-        <v>1</v>
-      </c>
-      <c r="X2" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="5">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="5">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="6">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="4">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="5">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="6">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
-      <c r="G3" s="6">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4">
-        <v>2</v>
-      </c>
-      <c r="I3" s="5">
-        <v>2</v>
-      </c>
-      <c r="J3" s="6">
-        <v>2</v>
-      </c>
-      <c r="K3" s="4">
-        <v>2</v>
-      </c>
-      <c r="L3" s="5">
-        <v>2</v>
-      </c>
-      <c r="M3" s="6">
-        <v>2</v>
-      </c>
-      <c r="N3" s="4">
-        <v>2</v>
-      </c>
-      <c r="O3" s="5">
-        <v>2</v>
-      </c>
-      <c r="P3" s="6">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>2</v>
-      </c>
-      <c r="R3" s="5">
-        <v>2</v>
-      </c>
-      <c r="S3" s="6">
-        <v>2</v>
-      </c>
-      <c r="T3" s="4">
-        <v>2</v>
-      </c>
-      <c r="U3" s="5">
-        <v>2</v>
-      </c>
-      <c r="V3" s="6">
-        <v>2</v>
-      </c>
-      <c r="W3" s="4">
-        <v>2</v>
-      </c>
-      <c r="X3" s="5">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>2</v>
-      </c>
-      <c r="AC3" s="3">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AF3" s="6">
-        <v>2</v>
-      </c>
-      <c r="AG3" s="3">
-        <v>2</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="6">
-        <v>2</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>2</v>
-      </c>
-      <c r="AL3" s="4">
-        <v>2</v>
-      </c>
-      <c r="AM3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AN3" s="6">
-        <v>2</v>
-      </c>
-      <c r="AO3" s="3">
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
         <v>2</v>
       </c>
     </row>
@@ -30876,7 +30952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:EW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EJ1" workbookViewId="0">
+    <sheetView topLeftCell="EJ1" workbookViewId="0">
       <selection activeCell="CY2" sqref="CY2:EW3"/>
     </sheetView>
   </sheetViews>

</xml_diff>